<commit_message>
Graf ide, Voting ide, Problems ide
</commit_message>
<xml_diff>
--- a/pm_projekt/src/graf.xlsx
+++ b/pm_projekt/src/graf.xlsx
@@ -1,31 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matejscislak/Desktop/4roc_ZS/PM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matejscislak/Desktop/4roc_ZS/PM/apka/ProjektManazment/pm_projekt/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A81389BC-A6FC-6B4A-B172-763F2EAE6A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0F6324-4E61-1E47-8335-5A59F482C1F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{ADCDBEAC-DD05-4B2E-8C0A-752D642F5F76}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15660" xr2:uid="{ADCDBEAC-DD05-4B2E-8C0A-752D642F5F76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="JAN" sheetId="2" r:id="rId2"/>
-    <sheet name="FEB" sheetId="4" r:id="rId3"/>
-    <sheet name="MAR" sheetId="5" r:id="rId4"/>
-    <sheet name="APR" sheetId="7" r:id="rId5"/>
-    <sheet name="MAJ" sheetId="8" r:id="rId6"/>
-    <sheet name="JUN" sheetId="9" r:id="rId7"/>
-    <sheet name="JUL" sheetId="10" r:id="rId8"/>
-    <sheet name="AUG" sheetId="11" r:id="rId9"/>
-    <sheet name="SEP" sheetId="12" r:id="rId10"/>
-    <sheet name="OCT" sheetId="13" r:id="rId11"/>
-    <sheet name="NOV" sheetId="14" r:id="rId12"/>
-    <sheet name="DEC" sheetId="15" r:id="rId13"/>
+    <sheet name="JAN_24" sheetId="2" r:id="rId2"/>
+    <sheet name="FEB_24" sheetId="4" r:id="rId3"/>
+    <sheet name="MAR_24" sheetId="5" r:id="rId4"/>
+    <sheet name="APR_24" sheetId="7" r:id="rId5"/>
+    <sheet name="MAJ_24" sheetId="8" r:id="rId6"/>
+    <sheet name="JUN_24" sheetId="9" r:id="rId7"/>
+    <sheet name="JUL_24" sheetId="10" r:id="rId8"/>
+    <sheet name="AUG_24" sheetId="11" r:id="rId9"/>
+    <sheet name="SEP_24" sheetId="12" r:id="rId10"/>
+    <sheet name="OCT_24" sheetId="13" r:id="rId11"/>
+    <sheet name="NOV_24" sheetId="14" r:id="rId12"/>
+    <sheet name="DEC_24" sheetId="15" r:id="rId13"/>
+    <sheet name="JAN_25" sheetId="16" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="47">
   <si>
     <t>Mesiac</t>
   </si>
@@ -56,42 +57,6 @@
     <t>Stav na ucte</t>
   </si>
   <si>
-    <t>January</t>
-  </si>
-  <si>
-    <t>February</t>
-  </si>
-  <si>
-    <t>March</t>
-  </si>
-  <si>
-    <t>April</t>
-  </si>
-  <si>
-    <t>May</t>
-  </si>
-  <si>
-    <t>June</t>
-  </si>
-  <si>
-    <t>July</t>
-  </si>
-  <si>
-    <t>August</t>
-  </si>
-  <si>
-    <t>September</t>
-  </si>
-  <si>
-    <t>October</t>
-  </si>
-  <si>
-    <t>November</t>
-  </si>
-  <si>
-    <t>December</t>
-  </si>
-  <si>
     <t>Vydaj</t>
   </si>
   <si>
@@ -147,6 +112,84 @@
   </si>
   <si>
     <t>AP</t>
+  </si>
+  <si>
+    <t>1_2024</t>
+  </si>
+  <si>
+    <t>2_2024</t>
+  </si>
+  <si>
+    <t>3_2024</t>
+  </si>
+  <si>
+    <t>4_2024</t>
+  </si>
+  <si>
+    <t>5_2024</t>
+  </si>
+  <si>
+    <t>6_2024</t>
+  </si>
+  <si>
+    <t>7_2024</t>
+  </si>
+  <si>
+    <t>8_2024</t>
+  </si>
+  <si>
+    <t>9_2024</t>
+  </si>
+  <si>
+    <t>10_2024</t>
+  </si>
+  <si>
+    <t>11_2024</t>
+  </si>
+  <si>
+    <t>12_2024</t>
+  </si>
+  <si>
+    <t>1_2025</t>
+  </si>
+  <si>
+    <t>Jan_2024</t>
+  </si>
+  <si>
+    <t>Feb_2024</t>
+  </si>
+  <si>
+    <t>Mar_2024</t>
+  </si>
+  <si>
+    <t>Máj_2024</t>
+  </si>
+  <si>
+    <t>Jún_2024</t>
+  </si>
+  <si>
+    <t>Júl_2024</t>
+  </si>
+  <si>
+    <t>Aug_2024</t>
+  </si>
+  <si>
+    <t>Sep_2024</t>
+  </si>
+  <si>
+    <t>Okt_2024</t>
+  </si>
+  <si>
+    <t>Nov_2024</t>
+  </si>
+  <si>
+    <t>Apr_2024</t>
+  </si>
+  <si>
+    <t>Dec_2024</t>
+  </si>
+  <si>
+    <t>Jan_2025</t>
   </si>
 </sst>
 </file>
@@ -249,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -270,6 +313,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,59 +422,62 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$13</c:f>
+              <c:f>Sheet1!$A$2:$A$17</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>January</c:v>
+                  <c:v>Jan_2024</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>February</c:v>
+                  <c:v>Feb_2024</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>March</c:v>
+                  <c:v>Mar_2024</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>April</c:v>
+                  <c:v>Apr_2024</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>May</c:v>
+                  <c:v>Máj_2024</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>June</c:v>
+                  <c:v>Jún_2024</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>July</c:v>
+                  <c:v>Júl_2024</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>August</c:v>
+                  <c:v>Aug_2024</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>September</c:v>
+                  <c:v>Sep_2024</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>October</c:v>
+                  <c:v>Okt_2024</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>November</c:v>
+                  <c:v>Nov_2024</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>December</c:v>
+                  <c:v>Dec_2024</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Jan_2025</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$13</c:f>
+              <c:f>Sheet1!$B$2:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>500</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>220</c:v>
@@ -460,6 +508,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>800</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1524,10 +1575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1712AACD-9C8B-4CD1-98F5-6067B36E85D7}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1536,7 +1587,7 @@
     <col min="2" max="2" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1544,112 +1595,160 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="B2">
-        <f>JAN!F2</f>
+        <f>JAN_24!F2</f>
         <v>800</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>3</v>
+      <c r="I2" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="B3">
-        <f>FEB!F2</f>
+        <f>FEB_24!F2</f>
+        <v>600</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <f>MAR_24!F2</f>
+        <v>220</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5">
+        <f>APR_24!F2</f>
         <v>500</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <f>MAR!F2</f>
-        <v>220</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <f>APR!F2</f>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>6</v>
+      <c r="I5" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="B6">
-        <f>MAJ!F2</f>
+        <f>MAJ_24!F2</f>
         <v>900</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>7</v>
+      <c r="I6" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="B7">
-        <f>JUN!F2</f>
+        <f>JUN_24!F2</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>8</v>
+      <c r="I7" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="B8">
-        <f>JUL!F2</f>
+        <f>JUL_24!F2</f>
         <v>140</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>9</v>
+      <c r="I8" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="B9">
-        <f>AUG!F2</f>
+        <f>AUG_24!F2</f>
         <v>1600</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>10</v>
+      <c r="I9" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="B10">
-        <f>SEP!F2</f>
+        <f>SEP_24!F2</f>
         <v>1900</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>11</v>
+      <c r="I10" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="B11">
-        <f>OCT!F2</f>
+        <f>OCT_24!F2</f>
         <v>1100</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>12</v>
+      <c r="I11" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="B12">
-        <f>NOV!F2</f>
+        <f>NOV_24!F2</f>
         <v>300</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>13</v>
+      <c r="I12" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="B13">
-        <f>DEC!F2</f>
+        <f>DEC_24!F2</f>
         <v>700</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14">
+        <f>JAN_24!F2</f>
+        <v>800</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1680,20 +1779,20 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="4" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1701,13 +1800,13 @@
         <v>100</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F2" s="5">
         <f>SUM(B:B) - SUM(A:A)</f>
@@ -1719,13 +1818,13 @@
         <v>500</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1733,55 +1832,55 @@
         <v>200</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B5" s="5">
         <v>200</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5">
         <v>700</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B7" s="5">
         <v>1800</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1810,20 +1909,20 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="4" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1831,13 +1930,13 @@
         <v>100</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F2" s="5">
         <f>SUM(B:B) - SUM(A:A)</f>
@@ -1849,13 +1948,13 @@
         <v>500</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1863,55 +1962,55 @@
         <v>200</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B5" s="5">
         <v>200</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5">
         <v>700</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B7" s="5">
         <v>1000</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1940,20 +2039,20 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="4" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1961,13 +2060,13 @@
         <v>100</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F2" s="5">
         <f>SUM(B:B) - SUM(A:A)</f>
@@ -1979,13 +2078,13 @@
         <v>500</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1993,55 +2092,55 @@
         <v>100</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B5" s="5">
         <v>200</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5">
         <v>700</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B7" s="5">
         <v>100</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2070,20 +2169,20 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="4" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2091,13 +2190,13 @@
         <v>100</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F2" s="5">
         <f>SUM(B:B) - SUM(A:A)</f>
@@ -2109,13 +2208,13 @@
         <v>500</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2123,55 +2222,185 @@
         <v>200</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B5" s="5">
         <v>200</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5">
         <v>1200</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B7" s="5">
         <v>100</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>31</v>
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{737AED56-17E5-3748-A9C8-E40E35045767}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.1640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="10" style="5" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="5"/>
+    <col min="6" max="6" width="17.83203125" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="9.1640625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>100</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="5">
+        <f>SUM(B:B) - SUM(A:A)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>500</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>200</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5">
+        <v>200</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="5">
+        <v>600</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5">
+        <v>100</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2200,20 +2429,20 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="4" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2221,13 +2450,13 @@
         <v>100</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F2" s="5">
         <f>SUM(B:B) - SUM(A:A)</f>
@@ -2239,13 +2468,13 @@
         <v>800</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2253,55 +2482,55 @@
         <v>200</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B5" s="5">
         <v>200</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5">
         <v>700</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B7" s="5">
         <v>1000</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2314,7 +2543,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2330,20 +2559,20 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="4" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2351,17 +2580,17 @@
         <v>100</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F2" s="5">
         <f>SUM(B:B) - SUM(A:A)</f>
-        <v>500</v>
+        <v>600</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2369,13 +2598,13 @@
         <v>50</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2383,55 +2612,55 @@
         <v>200</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B5" s="5">
         <v>50</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5">
         <v>700</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5">
+        <v>200</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="B7" s="5">
-        <v>100</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2460,20 +2689,20 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="4" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2481,13 +2710,13 @@
         <v>80</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F2" s="5">
         <f>SUM(B:B) - SUM(A:A)</f>
@@ -2499,13 +2728,13 @@
         <v>500</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2513,55 +2742,55 @@
         <v>200</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B5" s="5">
         <v>200</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5">
         <v>700</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B7" s="5">
         <v>100</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2590,20 +2819,20 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="4" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2611,13 +2840,13 @@
         <v>100</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F2" s="5">
         <f>SUM(B:B) - SUM(A:A)</f>
@@ -2629,13 +2858,13 @@
         <v>500</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2643,55 +2872,55 @@
         <v>200</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B5" s="5">
         <v>200</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5">
         <v>700</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B7" s="5">
         <v>400</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2703,9 +2932,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265F22A5-7E5E-4BB9-80C8-470C8A31A40B}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
-    </sheetView>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2720,20 +2947,20 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="4" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2741,13 +2968,13 @@
         <v>100</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F2" s="5">
         <f>SUM(B:B) - SUM(A:A)</f>
@@ -2759,13 +2986,13 @@
         <v>500</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2773,55 +3000,55 @@
         <v>200</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B5" s="5">
         <v>200</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5">
         <v>700</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B7" s="5">
         <v>800</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2850,20 +3077,20 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="4" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2871,13 +3098,13 @@
         <v>100</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F2" s="5">
         <f>SUM(B:B) - SUM(A:A)</f>
@@ -2889,13 +3116,13 @@
         <v>500</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2903,55 +3130,55 @@
         <v>400</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B5" s="5">
         <v>200</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5">
         <v>700</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B7" s="5">
         <v>100</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2980,20 +3207,20 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="4" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -3001,13 +3228,13 @@
         <v>60</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F2" s="5">
         <f>SUM(B:B) - SUM(A:A)</f>
@@ -3019,13 +3246,13 @@
         <v>500</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -3033,55 +3260,55 @@
         <v>200</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B5" s="5">
         <v>200</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5">
         <v>600</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B7" s="5">
         <v>100</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -3110,20 +3337,20 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="4" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -3131,13 +3358,13 @@
         <v>100</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F2" s="5">
         <f>SUM(B:B) - SUM(A:A)</f>
@@ -3149,13 +3376,13 @@
         <v>500</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -3163,55 +3390,55 @@
         <v>200</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B5" s="5">
         <v>200</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5">
         <v>700</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B7" s="5">
         <v>1500</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
verzia z dna 14.1.25 = obhajoba
</commit_message>
<xml_diff>
--- a/pm_projekt/src/graf.xlsx
+++ b/pm_projekt/src/graf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matejscislak/Desktop/4roc_ZS/PM/apka/ProjektManazment/pm_projekt/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0F6324-4E61-1E47-8335-5A59F482C1F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7A610B-CD02-0444-AB3B-8E9C890996E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15660" xr2:uid="{ADCDBEAC-DD05-4B2E-8C0A-752D642F5F76}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15660" activeTab="13" xr2:uid="{ADCDBEAC-DD05-4B2E-8C0A-752D642F5F76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="60">
   <si>
     <t>Mesiac</t>
   </si>
@@ -190,6 +190,45 @@
   </si>
   <si>
     <t>Jan_2025</t>
+  </si>
+  <si>
+    <t>rozbite dvere</t>
+  </si>
+  <si>
+    <t>benzin</t>
+  </si>
+  <si>
+    <t>zbierka</t>
+  </si>
+  <si>
+    <t>pozicka</t>
+  </si>
+  <si>
+    <t>poistenie dveri</t>
+  </si>
+  <si>
+    <t>1.1.2025</t>
+  </si>
+  <si>
+    <t>5.1.2025</t>
+  </si>
+  <si>
+    <t>7.1.2025</t>
+  </si>
+  <si>
+    <t>10.1.2025</t>
+  </si>
+  <si>
+    <t>16.1.2025</t>
+  </si>
+  <si>
+    <t>26.1.2025</t>
+  </si>
+  <si>
+    <t>30.1.2025</t>
+  </si>
+  <si>
+    <t>kupa kosacky</t>
   </si>
 </sst>
 </file>
@@ -483,7 +522,7 @@
                   <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>500</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>900</c:v>
@@ -510,7 +549,7 @@
                   <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>800</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1577,8 +1616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1712AACD-9C8B-4CD1-98F5-6067B36E85D7}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1637,7 +1676,7 @@
       </c>
       <c r="B5">
         <f>APR_24!F2</f>
-        <v>500</v>
+        <v>900</v>
       </c>
       <c r="I5" s="9" t="s">
         <v>24</v>
@@ -1744,8 +1783,8 @@
         <v>46</v>
       </c>
       <c r="B14">
-        <f>JAN_24!F2</f>
-        <v>800</v>
+        <f>JAN_25!F2</f>
+        <v>300</v>
       </c>
       <c r="I14" s="9" t="s">
         <v>33</v>
@@ -2280,10 +2319,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{737AED56-17E5-3748-A9C8-E40E35045767}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2299,7 +2338,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -2317,48 +2356,48 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="5">
         <f>SUM(B:B) - SUM(A:A)</f>
-        <v>100</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -2366,13 +2405,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="5">
-        <v>200</v>
+        <v>1500</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -2380,13 +2419,13 @@
         <v>7</v>
       </c>
       <c r="B6" s="5">
-        <v>600</v>
+        <v>1700</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -2394,13 +2433,27 @@
         <v>7</v>
       </c>
       <c r="B7" s="5">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>19</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>650</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2803,7 +2856,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2850,7 +2903,7 @@
       </c>
       <c r="F2" s="5">
         <f>SUM(B:B) - SUM(A:A)</f>
-        <v>500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2914,7 +2967,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="5">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>13</v>

</xml_diff>